<commit_message>
blind unsensitive SIMAT 2017
</commit_message>
<xml_diff>
--- a/data/_metadata/dicts/tables.xlsx
+++ b/data/_metadata/dicts/tables.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajoseguerrero/Documents/Secretaria de Educación/Deserción Escolar/school_dropout/data/_metadata/dicts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juanrengifo101/Documents/_trabajo/IDEA/school_dropout/data/_metadata/dicts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C9B3CF-A31E-2844-B15B-D5CC9CD3AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182AF335-E8FE-2D4B-9D16-4EB8AF149685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tablas" sheetId="4" r:id="rId1"/>
     <sheet name="Clasificacion" sheetId="5" r:id="rId2"/>
-    <sheet name="TIPO_DOCUMENTO_ids_map" sheetId="6" r:id="rId3"/>
-    <sheet name="resumen" sheetId="3" r:id="rId4"/>
+    <sheet name="TIPO_DOCUMENTO_ids_map_2004" sheetId="6" r:id="rId3"/>
+    <sheet name="TIPO_DOCUMENTO_ids_map_2017" sheetId="7" r:id="rId4"/>
+    <sheet name="resumen" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="226">
   <si>
     <t>2004 MATRICULA VALIDADA_Hoja1.parquet</t>
   </si>
@@ -1111,6 +1112,12 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,12 +1144,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1568,30 +1569,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>211</v>
       </c>
-      <c r="C1" s="38"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="24"/>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="36"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="38"/>
       <c r="W1" s="24"/>
     </row>
     <row r="2" spans="2:23" x14ac:dyDescent="0.2">
@@ -2601,11 +2602,11 @@
       </c>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B38" s="39" t="s">
+      <c r="B38" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="40"/>
-      <c r="D38" s="41"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="43"/>
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.2">
@@ -3023,24 +3024,24 @@
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B79" s="42"/>
-      <c r="C79" s="42"/>
+      <c r="B79" s="44"/>
+      <c r="C79" s="44"/>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B80" s="42"/>
-      <c r="C80" s="42"/>
+      <c r="B80" s="44"/>
+      <c r="C80" s="44"/>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B81" s="42"/>
-      <c r="C81" s="42"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="44"/>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B82" s="42"/>
-      <c r="C82" s="42"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="44"/>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B83" s="42"/>
-      <c r="C83" s="42"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -3353,17 +3354,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36A7A0CD-CDC1-4B45-AC71-95F22D6BC89F}">
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="34" t="s">
         <v>212</v>
       </c>
     </row>
@@ -3371,7 +3372,7 @@
       <c r="A2" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="35" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3379,7 +3380,7 @@
       <c r="A3" t="s">
         <v>87</v>
       </c>
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="35" t="s">
         <v>87</v>
       </c>
     </row>
@@ -3387,7 +3388,7 @@
       <c r="A4" t="s">
         <v>84</v>
       </c>
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="35" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3395,7 +3396,7 @@
       <c r="A5" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="35" t="s">
         <v>79</v>
       </c>
     </row>
@@ -3403,7 +3404,7 @@
       <c r="A6" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="35" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3411,7 +3412,7 @@
       <c r="A7" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="35" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3419,7 +3420,7 @@
       <c r="A8" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="35" t="s">
         <v>86</v>
       </c>
     </row>
@@ -3427,7 +3428,7 @@
       <c r="A9" t="s">
         <v>89</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="35" t="s">
         <v>89</v>
       </c>
     </row>
@@ -3435,7 +3436,7 @@
       <c r="A10" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="35" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3443,7 +3444,7 @@
       <c r="A11" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="35" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3451,7 +3452,7 @@
       <c r="A12" t="s">
         <v>82</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="35" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3459,7 +3460,7 @@
       <c r="A13" t="s">
         <v>213</v>
       </c>
-      <c r="B13" s="44">
+      <c r="B13" s="35">
         <v>5</v>
       </c>
     </row>
@@ -3467,7 +3468,7 @@
       <c r="A14" t="s">
         <v>214</v>
       </c>
-      <c r="B14" s="44">
+      <c r="B14" s="35">
         <v>2</v>
       </c>
     </row>
@@ -3475,7 +3476,7 @@
       <c r="A15" t="s">
         <v>215</v>
       </c>
-      <c r="B15" s="44">
+      <c r="B15" s="35">
         <v>7</v>
       </c>
     </row>
@@ -3483,7 +3484,7 @@
       <c r="A16" t="s">
         <v>216</v>
       </c>
-      <c r="B16" s="44">
+      <c r="B16" s="35">
         <v>-1</v>
       </c>
     </row>
@@ -3491,7 +3492,7 @@
       <c r="A17" t="s">
         <v>217</v>
       </c>
-      <c r="B17" s="44">
+      <c r="B17" s="35">
         <v>1</v>
       </c>
     </row>
@@ -3499,7 +3500,7 @@
       <c r="A18" t="s">
         <v>218</v>
       </c>
-      <c r="B18" s="44">
+      <c r="B18" s="35">
         <v>9</v>
       </c>
     </row>
@@ -3507,7 +3508,7 @@
       <c r="A19" t="s">
         <v>219</v>
       </c>
-      <c r="B19" s="44">
+      <c r="B19" s="35">
         <v>3</v>
       </c>
     </row>
@@ -3515,7 +3516,7 @@
       <c r="A20" t="s">
         <v>220</v>
       </c>
-      <c r="B20" s="44">
+      <c r="B20" s="35">
         <v>6</v>
       </c>
     </row>
@@ -3523,7 +3524,7 @@
       <c r="A21" t="s">
         <v>83</v>
       </c>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="35" t="s">
         <v>83</v>
       </c>
     </row>
@@ -3531,7 +3532,7 @@
       <c r="A22" t="s">
         <v>221</v>
       </c>
-      <c r="B22" s="44">
+      <c r="B22" s="35">
         <v>-2</v>
       </c>
     </row>
@@ -3539,7 +3540,7 @@
       <c r="A23" t="s">
         <v>222</v>
       </c>
-      <c r="B23" s="44">
+      <c r="B23" s="35">
         <v>-1</v>
       </c>
     </row>
@@ -3547,7 +3548,7 @@
       <c r="A24" t="s">
         <v>223</v>
       </c>
-      <c r="B24" s="44">
+      <c r="B24" s="35">
         <v>-2</v>
       </c>
     </row>
@@ -3555,7 +3556,7 @@
       <c r="A25" t="s">
         <v>224</v>
       </c>
-      <c r="B25" s="44">
+      <c r="B25" s="35">
         <v>7</v>
       </c>
     </row>
@@ -3563,7 +3564,7 @@
       <c r="A26" t="s">
         <v>225</v>
       </c>
-      <c r="B26" s="44">
+      <c r="B26" s="35">
         <v>6</v>
       </c>
     </row>
@@ -3573,6 +3574,104 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1DECE9C-42B6-694C-A887-79AE6A38AEA6}">
+  <dimension ref="A1:B26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="35"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="35"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="35"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="35"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="35"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="35"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B8" s="35"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B9" s="35"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="35"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="35"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B12" s="35"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="35"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B14" s="35"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="35"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="35"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="35"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="35"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="35"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="35"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="35"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="35"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="35"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="35"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="35"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1435D5A1-0AC9-6D49-8B79-0AC50D35E22C}">
   <dimension ref="B2:N12"/>
   <sheetViews>

</xml_diff>